<commit_message>
completed codingfor db access
</commit_message>
<xml_diff>
--- a/src/main/resources/fm/spec/form/form1.xlsx
+++ b/src/main/resources/fm/spec/form/form1.xlsx
@@ -18,14 +18,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhZV/KAG9TuY2/gdm5uOblSXwWzEw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhNlzoCWtbU6Rp8fsXgYi7eWJoIJg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="184">
   <si>
     <t>Sheet</t>
   </si>
@@ -39,16 +39,13 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>references to otherdocuments ofrelevance to this form</t>
-  </si>
-  <si>
     <t>DO NOT DELETE ANY SHEET OR ROW HEADERS IN ANY SHEET</t>
   </si>
   <si>
     <t>All notes,including Q&amp;A about this form</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
   <si>
     <t>(entire book)</t>
@@ -59,6 +56,9 @@
 Project team should decide how this is initiated/developed/reviewed/approved.
 Once approved, it becomes part of the project artifact, and is included in the resource folder of the project.
 </t>
+  </si>
+  <si>
+    <t>references to otherdocuments ofrelevance to this form</t>
   </si>
   <si>
     <t xml:space="preserve">     notes</t>
@@ -143,6 +143,20 @@
   </si>
   <si>
     <t>any special processing logic to be implemented AFTER submitting the form? description is provided by BA. programmers provides the java class name as value in the previous cell</t>
+  </si>
+  <si>
+    <t>dbTableName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of a table or view in the rdbms that is linked to this form. This is used to manage persistence </t>
+  </si>
+  <si>
+    <t>dbKeyFields</t>
+  </si>
+  <si>
+    <t>comma separated name of fields in this form that together form the primary key for the table.
+Note that these are name of form fields, and NOT data base column names. db column names 
+are picked from fields sheet</t>
   </si>
   <si>
     <t>fields</t>
@@ -249,6 +263,12 @@
     <t>If the value list is fixed, like all the countries, then this column is not required.
 If the value list depends on one the value of another field, specify the name of the field in this form
 that has the value for the key. For example put contryCode as the value list key field name for stateCode vaulelist</t>
+  </si>
+  <si>
+    <t>dbColumnName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of the column the table to which this field is linked to. </t>
   </si>
   <si>
     <t>childForms</t>
@@ -378,6 +398,9 @@
     <t>addCommonFields</t>
   </si>
   <si>
+    <t>should common fields (defined in commonFields sheet in application.slsx workbook ) be inserted into this form.</t>
+  </si>
+  <si>
     <t>Is Editable</t>
   </si>
   <si>
@@ -385,6 +408,9 @@
   </si>
   <si>
     <t>customerId</t>
+  </si>
+  <si>
+    <t>Db Column Name</t>
   </si>
   <si>
     <t>Customer Id</t>
@@ -396,13 +422,31 @@
     <t>customer id</t>
   </si>
   <si>
-    <t>should common fields (defined in commonFields sheet in application.slsx workbook ) be inserted into this form.</t>
+    <t>createGetService</t>
+  </si>
+  <si>
+    <t>if set to true, this form can be requested reading by the client</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>createSaveService</t>
+  </si>
+  <si>
+    <t>if set to true, client can send data to be saved (not submit)</t>
+  </si>
+  <si>
+    <t>createSubmitService</t>
   </si>
   <si>
     <t>financialYear</t>
   </si>
   <si>
     <t>Financial Year</t>
+  </si>
+  <si>
+    <t>if set totrue, client send data forsave and submit</t>
   </si>
   <si>
     <t>FInancial year</t>
@@ -414,22 +458,10 @@
     <t>fy</t>
   </si>
   <si>
-    <t>createGetService</t>
+    <t>if saveis allowed, and this is set to true,client can send a subset of teh form fields, say a section, for saving (not for submit.Submit always requires all fields)</t>
   </si>
   <si>
-    <t>if set to true, this form can be requested reading by the client</t>
-  </si>
-  <si>
-    <t>createSaveService</t>
-  </si>
-  <si>
-    <t>if set to true, client can send data to be saved (not submit)</t>
-  </si>
-  <si>
-    <t>createSubmitService</t>
-  </si>
-  <si>
-    <t>if set totrue, client send data forsave and submit</t>
+    <t>financial_year</t>
   </si>
   <si>
     <t>boolField</t>
@@ -441,10 +473,16 @@
     <t>some boolean field</t>
   </si>
   <si>
+    <t>MyPreGet</t>
+  </si>
+  <si>
     <t>boolean field</t>
   </si>
   <si>
     <t>trueFalse</t>
+  </si>
+  <si>
+    <t>bool_field</t>
   </si>
   <si>
     <t>fromDate</t>
@@ -459,10 +497,13 @@
     <t>from field</t>
   </si>
   <si>
-    <t>if saveis allowed, and this is set to true,client can send a subset of teh form fields, say a section, for saving (not for submit.Submit always requires all fields)</t>
+    <t>futureDate</t>
   </si>
   <si>
-    <t>futureDate</t>
+    <t>MyPostGet</t>
+  </si>
+  <si>
+    <t>from_date</t>
   </si>
   <si>
     <t>toDate</t>
@@ -477,7 +518,7 @@
     <t>to field</t>
   </si>
   <si>
-    <t>MyPreGet</t>
+    <t>to_date</t>
   </si>
   <si>
     <t>intField1</t>
@@ -492,7 +533,7 @@
     <t>qty</t>
   </si>
   <si>
-    <t>MyPostGet</t>
+    <t>int_field1</t>
   </si>
   <si>
     <t>intField2</t>
@@ -502,6 +543,9 @@
   </si>
   <si>
     <t>int field 2</t>
+  </si>
+  <si>
+    <t>int_field2</t>
   </si>
   <si>
     <t>derivedField</t>
@@ -520,6 +564,18 @@
   </si>
   <si>
     <t>current FY</t>
+  </si>
+  <si>
+    <t>test_table</t>
+  </si>
+  <si>
+    <t>this can be a view if it meant only for read.</t>
+  </si>
+  <si>
+    <t>customerId,financialYear</t>
+  </si>
+  <si>
+    <t>comma separated list of field names (these must be defined in fields sheet) that together work as primary key on the table</t>
   </si>
   <si>
     <t>fieldName</t>
@@ -550,9 +606,6 @@
   </si>
   <si>
     <t>Equal Value Ok</t>
-  </si>
-  <si>
-    <t>fromdate</t>
   </si>
   <si>
     <t>invalidDateRange</t>
@@ -650,15 +703,15 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -766,7 +819,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -794,11 +847,11 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1330,8 +1383,12 @@
     </row>
     <row r="20">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1358,8 +1415,12 @@
     </row>
     <row r="21">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1385,13 +1446,9 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1417,12 +1474,12 @@
       <c r="Z22" s="5"/>
     </row>
     <row r="23">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
-        <v>40</v>
+      <c r="A23" s="3" t="s">
+        <v>42</v>
       </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1451,10 +1508,10 @@
     <row r="24">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1483,10 +1540,10 @@
     <row r="25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1515,10 +1572,10 @@
     <row r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1547,10 +1604,10 @@
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1579,10 +1636,10 @@
     <row r="28">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1611,10 +1668,10 @@
     <row r="29">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1643,10 +1700,10 @@
     <row r="30">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1675,10 +1732,10 @@
     <row r="31">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1707,10 +1764,10 @@
     <row r="32">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1739,10 +1796,10 @@
     <row r="33">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1770,11 +1827,11 @@
     </row>
     <row r="34">
       <c r="A34" s="3"/>
-      <c r="B34" s="6" t="s">
-        <v>62</v>
+      <c r="B34" s="3" t="s">
+        <v>64</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>63</v>
+      <c r="C34" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -1803,10 +1860,10 @@
     <row r="35">
       <c r="A35" s="3"/>
       <c r="B35" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1834,8 +1891,12 @@
     </row>
     <row r="36">
       <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="B36" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1862,8 +1923,12 @@
     </row>
     <row r="37">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1889,13 +1954,9 @@
       <c r="Z37" s="5"/>
     </row>
     <row r="38">
-      <c r="A38" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1921,12 +1982,12 @@
       <c r="Z38" s="5"/>
     </row>
     <row r="39">
-      <c r="A39" s="3"/>
-      <c r="B39" s="6" t="s">
-        <v>40</v>
+      <c r="A39" s="6" t="s">
+        <v>72</v>
       </c>
+      <c r="B39" s="3"/>
       <c r="C39" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -1955,10 +2016,10 @@
     <row r="40">
       <c r="A40" s="3"/>
       <c r="B40" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1986,11 +2047,11 @@
     </row>
     <row r="41">
       <c r="A41" s="3"/>
-      <c r="B41" s="3" t="s">
-        <v>70</v>
+      <c r="B41" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -2019,10 +2080,10 @@
     <row r="42">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2051,10 +2112,10 @@
     <row r="43">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -2082,11 +2143,11 @@
     </row>
     <row r="44">
       <c r="A44" s="3"/>
-      <c r="B44" s="6" t="s">
-        <v>52</v>
+      <c r="B44" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2114,8 +2175,12 @@
     </row>
     <row r="45">
       <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="B45" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -2141,13 +2206,9 @@
       <c r="Z45" s="5"/>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -2173,12 +2234,12 @@
       <c r="Z46" s="5"/>
     </row>
     <row r="47">
-      <c r="A47" s="8"/>
-      <c r="B47" s="6" t="s">
-        <v>79</v>
+      <c r="A47" s="6" t="s">
+        <v>83</v>
       </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -2205,12 +2266,12 @@
       <c r="Z47" s="5"/>
     </row>
     <row r="48">
-      <c r="A48" s="3"/>
+      <c r="A48" s="8"/>
       <c r="B48" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -2239,10 +2300,10 @@
     <row r="49">
       <c r="A49" s="3"/>
       <c r="B49" s="6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -2270,11 +2331,11 @@
     </row>
     <row r="50">
       <c r="A50" s="3"/>
-      <c r="B50" s="3" t="s">
-        <v>52</v>
+      <c r="B50" s="6" t="s">
+        <v>87</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>83</v>
+      <c r="C50" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -2302,8 +2363,12 @@
     </row>
     <row r="51">
       <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -2329,13 +2394,9 @@
       <c r="Z51" s="5"/>
     </row>
     <row r="52">
-      <c r="A52" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="A52" s="3"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="6" t="s">
-        <v>85</v>
-      </c>
+      <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -2361,12 +2422,12 @@
       <c r="Z52" s="5"/>
     </row>
     <row r="53">
-      <c r="A53" s="3"/>
-      <c r="B53" s="6" t="s">
-        <v>86</v>
+      <c r="A53" s="6" t="s">
+        <v>90</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>87</v>
+      <c r="B53" s="3"/>
+      <c r="C53" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -2394,11 +2455,11 @@
     </row>
     <row r="54">
       <c r="A54" s="3"/>
-      <c r="B54" s="3" t="s">
-        <v>88</v>
+      <c r="B54" s="6" t="s">
+        <v>92</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>89</v>
+      <c r="C54" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -2426,11 +2487,11 @@
     </row>
     <row r="55">
       <c r="A55" s="3"/>
-      <c r="B55" s="6" t="s">
-        <v>90</v>
+      <c r="B55" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -2458,11 +2519,11 @@
     </row>
     <row r="56">
       <c r="A56" s="3"/>
-      <c r="B56" s="3" t="s">
-        <v>52</v>
+      <c r="B56" s="6" t="s">
+        <v>96</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>83</v>
+      <c r="C56" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -2490,8 +2551,12 @@
     </row>
     <row r="57">
       <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -2517,72 +2582,68 @@
       <c r="Z57" s="5"/>
     </row>
     <row r="58">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
-      <c r="Q58" s="8"/>
-      <c r="R58" s="8"/>
-      <c r="S58" s="8"/>
-      <c r="T58" s="8"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="8"/>
-      <c r="W58" s="8"/>
-      <c r="X58" s="8"/>
-      <c r="Y58" s="8"/>
-      <c r="Z58" s="8"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
     </row>
     <row r="59">
-      <c r="A59" s="6" t="s">
-        <v>92</v>
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="8"/>
+      <c r="S59" s="8"/>
+      <c r="T59" s="8"/>
+      <c r="U59" s="8"/>
+      <c r="V59" s="8"/>
+      <c r="W59" s="8"/>
+      <c r="X59" s="8"/>
+      <c r="Y59" s="8"/>
+      <c r="Z59" s="8"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="s">
+        <v>98</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
-      <c r="S59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="5"/>
-      <c r="V59" s="5"/>
-      <c r="W59" s="5"/>
-      <c r="X59" s="5"/>
-      <c r="Y59" s="5"/>
-      <c r="Z59" s="5"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>87</v>
+      <c r="B60" s="3"/>
+      <c r="C60" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2610,11 +2671,11 @@
     </row>
     <row r="61">
       <c r="A61" s="3"/>
-      <c r="B61" s="6" t="s">
-        <v>95</v>
+      <c r="B61" s="3" t="s">
+        <v>100</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>96</v>
+      <c r="C61" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2643,10 +2704,10 @@
     <row r="62">
       <c r="A62" s="3"/>
       <c r="B62" s="6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2674,11 +2735,11 @@
     </row>
     <row r="63">
       <c r="A63" s="3"/>
-      <c r="B63" s="3" t="s">
-        <v>52</v>
+      <c r="B63" s="6" t="s">
+        <v>103</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>83</v>
+      <c r="C63" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -2706,8 +2767,12 @@
     </row>
     <row r="64">
       <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="B64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -2733,13 +2798,9 @@
       <c r="Z64" s="5"/>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="A65" s="3"/>
       <c r="B65" s="3"/>
-      <c r="C65" s="6" t="s">
-        <v>100</v>
-      </c>
+      <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -2765,9 +2826,13 @@
       <c r="Z65" s="5"/>
     </row>
     <row r="66">
-      <c r="A66" s="3"/>
+      <c r="A66" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+      <c r="C66" s="6" t="s">
+        <v>106</v>
+      </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -8113,26 +8178,26 @@
       <c r="Z256" s="5"/>
     </row>
     <row r="257">
-      <c r="A257" s="5"/>
-      <c r="B257" s="5"/>
-      <c r="C257" s="5"/>
-      <c r="D257" s="5"/>
-      <c r="E257" s="5"/>
-      <c r="F257" s="5"/>
-      <c r="G257" s="5"/>
-      <c r="H257" s="5"/>
-      <c r="I257" s="5"/>
-      <c r="J257" s="5"/>
-      <c r="K257" s="5"/>
-      <c r="L257" s="5"/>
-      <c r="M257" s="5"/>
-      <c r="N257" s="5"/>
-      <c r="O257" s="5"/>
-      <c r="P257" s="5"/>
-      <c r="Q257" s="5"/>
-      <c r="R257" s="5"/>
-      <c r="S257" s="5"/>
-      <c r="T257" s="5"/>
+      <c r="A257" s="3"/>
+      <c r="B257" s="3"/>
+      <c r="C257" s="3"/>
+      <c r="D257" s="3"/>
+      <c r="E257" s="3"/>
+      <c r="F257" s="3"/>
+      <c r="G257" s="3"/>
+      <c r="H257" s="3"/>
+      <c r="I257" s="3"/>
+      <c r="J257" s="3"/>
+      <c r="K257" s="3"/>
+      <c r="L257" s="3"/>
+      <c r="M257" s="3"/>
+      <c r="N257" s="3"/>
+      <c r="O257" s="3"/>
+      <c r="P257" s="3"/>
+      <c r="Q257" s="3"/>
+      <c r="R257" s="3"/>
+      <c r="S257" s="3"/>
+      <c r="T257" s="3"/>
       <c r="U257" s="5"/>
       <c r="V257" s="5"/>
       <c r="W257" s="5"/>
@@ -29504,6 +29569,34 @@
       <c r="Y1020" s="5"/>
       <c r="Z1020" s="5"/>
     </row>
+    <row r="1021">
+      <c r="A1021" s="5"/>
+      <c r="B1021" s="5"/>
+      <c r="C1021" s="5"/>
+      <c r="D1021" s="5"/>
+      <c r="E1021" s="5"/>
+      <c r="F1021" s="5"/>
+      <c r="G1021" s="5"/>
+      <c r="H1021" s="5"/>
+      <c r="I1021" s="5"/>
+      <c r="J1021" s="5"/>
+      <c r="K1021" s="5"/>
+      <c r="L1021" s="5"/>
+      <c r="M1021" s="5"/>
+      <c r="N1021" s="5"/>
+      <c r="O1021" s="5"/>
+      <c r="P1021" s="5"/>
+      <c r="Q1021" s="5"/>
+      <c r="R1021" s="5"/>
+      <c r="S1021" s="5"/>
+      <c r="T1021" s="5"/>
+      <c r="U1021" s="5"/>
+      <c r="V1021" s="5"/>
+      <c r="W1021" s="5"/>
+      <c r="X1021" s="5"/>
+      <c r="Y1021" s="5"/>
+      <c r="Z1021" s="5"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -29525,11 +29618,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>44</v>
+      <c r="B1" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -29537,7 +29630,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
@@ -30589,7 +30682,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -35995,7 +36088,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -36018,7 +36111,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -41415,20 +41508,20 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="26.86"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
+    <col customWidth="1" min="2" max="2" width="17.86"/>
     <col customWidth="1" min="3" max="3" width="92.29"/>
     <col customWidth="1" min="4" max="7" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>101</v>
+      <c r="A1" s="9" t="s">
+        <v>107</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>102</v>
+      <c r="B1" s="9" t="s">
+        <v>108</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>44</v>
+      <c r="C1" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -41449,13 +41542,13 @@
       <c r="T1" s="4"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>103</v>
+      <c r="A2" s="11" t="s">
+        <v>109</v>
       </c>
-      <c r="B2" s="12" t="b">
+      <c r="B2" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>110</v>
       </c>
       <c r="D2" s="4"/>
@@ -41477,13 +41570,13 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>106</v>
+      <c r="B3" s="11" t="s">
+        <v>113</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4"/>
@@ -41505,14 +41598,14 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="12" t="s">
-        <v>116</v>
+      <c r="A4" s="11" t="s">
+        <v>118</v>
       </c>
-      <c r="B4" s="12" t="b">
+      <c r="B4" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>117</v>
+      <c r="C4" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -41533,14 +41626,14 @@
       <c r="T4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>118</v>
+      <c r="A5" s="11" t="s">
+        <v>121</v>
       </c>
-      <c r="B5" s="12" t="b">
+      <c r="B5" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>119</v>
+      <c r="C5" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -41561,14 +41654,14 @@
       <c r="T5" s="4"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>120</v>
+      <c r="A6" s="11" t="s">
+        <v>123</v>
       </c>
-      <c r="B6" s="12" t="b">
+      <c r="B6" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>121</v>
+      <c r="C6" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -41589,14 +41682,14 @@
       <c r="T6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="12" t="b">
+      <c r="B7" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>131</v>
+      <c r="C7" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -41617,13 +41710,13 @@
       <c r="T7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>137</v>
+      <c r="B8" s="11" t="s">
+        <v>135</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="4"/>
@@ -41645,13 +41738,13 @@
       <c r="T8" s="4"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>142</v>
+      <c r="B9" s="11" t="s">
+        <v>144</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="4"/>
@@ -41673,11 +41766,11 @@
       <c r="T9" s="4"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4"/>
@@ -41699,11 +41792,11 @@
       <c r="T10" s="4"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="4"/>
@@ -41725,11 +41818,11 @@
       <c r="T11" s="4"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D12" s="4"/>
@@ -41751,11 +41844,11 @@
       <c r="T12" s="4"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="4"/>
@@ -41777,9 +41870,15 @@
       <c r="T13" s="4"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>167</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -41799,9 +41898,15 @@
       <c r="T14" s="4"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>169</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -47163,64 +47268,68 @@
     <col customWidth="1" min="11" max="11" width="11.0"/>
     <col customWidth="1" min="12" max="12" width="17.43"/>
     <col customWidth="1" min="13" max="13" width="24.29"/>
+    <col customWidth="1" min="14" max="14" width="23.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>104</v>
+      <c r="G1" s="12" t="s">
+        <v>56</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>60</v>
+      <c r="I1" s="10" t="s">
+        <v>111</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>105</v>
+      <c r="K1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="H2" s="13" t="b">
         <v>1</v>
@@ -47235,22 +47344,25 @@
         <v>1</v>
       </c>
       <c r="M2" s="13"/>
+      <c r="N2" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="F3" s="13"/>
       <c r="H3" s="13" t="b">
@@ -47266,22 +47378,25 @@
         <v>1</v>
       </c>
       <c r="M3" s="13"/>
+      <c r="N3" s="14" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="H4" s="13" t="b">
         <v>0</v>
@@ -47296,22 +47411,25 @@
         <v>0</v>
       </c>
       <c r="M4" s="13"/>
+      <c r="N4" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H5" s="13" t="b">
         <v>0</v>
@@ -47326,22 +47444,25 @@
         <v>0</v>
       </c>
       <c r="M5" s="13"/>
+      <c r="N5" s="14" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H6" s="13" t="b">
         <v>0</v>
@@ -47356,22 +47477,25 @@
         <v>0</v>
       </c>
       <c r="M6" s="13"/>
+      <c r="N6" s="14" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="F7" s="13">
         <v>33.0</v>
@@ -47389,22 +47513,25 @@
         <v>0</v>
       </c>
       <c r="M7" s="13"/>
+      <c r="N7" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="F8" s="13">
         <v>45.0</v>
@@ -47422,19 +47549,22 @@
         <v>0</v>
       </c>
       <c r="M8" s="13"/>
+      <c r="N8" s="14" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="H9" s="13" t="b">
         <v>0</v>
@@ -47452,16 +47582,16 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="H10" s="13" t="b">
         <v>0</v>
@@ -48489,37 +48619,37 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>152</v>
+      <c r="A1" s="12" t="s">
+        <v>170</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>42</v>
+      <c r="B1" s="12" t="s">
+        <v>46</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>70</v>
+      <c r="C1" s="10" t="s">
+        <v>76</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>153</v>
+      <c r="D1" s="12" t="s">
+        <v>171</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>72</v>
+      <c r="E1" s="10" t="s">
+        <v>78</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>74</v>
+      <c r="F1" s="10" t="s">
+        <v>80</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>154</v>
+      <c r="G1" s="12" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="D2" s="14" t="b">
         <v>1</v>
@@ -48531,7 +48661,7 @@
         <v>200.0</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
@@ -49554,31 +49684,31 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>159</v>
+      <c r="A1" s="10" t="s">
+        <v>177</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>160</v>
+      <c r="B1" s="10" t="s">
+        <v>178</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>161</v>
+      <c r="C1" s="10" t="s">
+        <v>179</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>52</v>
+      <c r="D1" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
-        <v>162</v>
+      <c r="A2" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="C2" s="13" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
@@ -50602,17 +50732,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>164</v>
+      <c r="A1" s="10" t="s">
+        <v>181</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>95</v>
+      <c r="B1" s="10" t="s">
+        <v>101</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>97</v>
+      <c r="C1" s="12" t="s">
+        <v>103</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>52</v>
+      <c r="D1" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -51636,17 +51766,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>164</v>
+      <c r="A1" s="10" t="s">
+        <v>181</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>88</v>
+      <c r="B1" s="10" t="s">
+        <v>94</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>165</v>
+      <c r="C1" s="12" t="s">
+        <v>182</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>52</v>
+      <c r="D1" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>

</xml_diff>